<commit_message>
Electricity sector file updates
</commit_message>
<xml_diff>
--- a/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
+++ b/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-EPS\InputData\elec\BPHC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/elec/BPHC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2701B040-E8F6-4B5E-87A7-9ED41B286E94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA08199-9104-EE4B-96AA-0DCE0D2EFAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="900" windowWidth="20265" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="900" windowWidth="20260" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="140">
   <si>
     <t>BPHC BAU Pumped Hydro Capacity</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>Energy Information Administration</t>
-  </si>
-  <si>
-    <t>Table 9, Row "Pumped Storage"</t>
-  </si>
-  <si>
     <t>9. Electricity Generating Capacity</t>
   </si>
   <si>
@@ -457,7 +451,10 @@
     <t>AEO2021 National Energy Modeling System run highogs.d120120a. Projections:  EIA, AEO2021 National Energy Modeling System run highogs.d120120a.</t>
   </si>
   <si>
-    <t>https://www.eia.gov/outlooks/aeo/tables_side.php</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>No pumped hydro capacity in Mexico</t>
   </si>
 </sst>
 </file>
@@ -525,6 +522,7 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -535,6 +533,7 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -673,11 +672,11 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="7" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1027,58 +1026,46 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B9" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -1098,15 +1085,15 @@
       <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="9">
         <v>2020</v>
@@ -1202,58 +1189,58 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -1261,26 +1248,26 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="10" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH10" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AH11" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1314,12 +1301,12 @@
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="9">
         <v>2020</v>
@@ -1415,26 +1402,26 @@
         <v>2050</v>
       </c>
       <c r="AH13" s="20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>9</v>
       </c>
       <c r="C17" s="13">
         <v>217.319931</v>
@@ -1533,12 +1520,12 @@
         <v>-3.5593E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" s="13">
         <v>72.645202999999995</v>
@@ -1637,12 +1624,12 @@
         <v>-1.1639E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" s="13">
         <v>245.41911300000001</v>
@@ -1741,12 +1728,12 @@
         <v>2.2079999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="13">
         <v>139.99884</v>
@@ -1845,12 +1832,12 @@
         <v>2.6945E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="13">
         <v>97.120911000000007</v>
@@ -1949,12 +1936,12 @@
         <v>-2.7585999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="24">
         <v>22.778303000000001</v>
@@ -2053,12 +2040,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="13">
         <v>3.1509999999999998</v>
@@ -2157,12 +2144,12 @@
         <v>5.9369999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="13">
         <v>0.20419999999999999</v>
@@ -2261,12 +2248,12 @@
         <v>4.4720000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="13">
         <v>263.93090799999999</v>
@@ -2365,12 +2352,12 @@
         <v>2.9822000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="13">
         <v>0</v>
@@ -2466,15 +2453,15 @@
         <v>36.505851999999997</v>
       </c>
       <c r="AH26" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="15">
         <v>1062.568481</v>
@@ -2573,17 +2560,17 @@
         <v>1.5070999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C29" s="13">
         <v>1.8878999999999999</v>
@@ -2682,12 +2669,12 @@
         <v>-1.9059999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="13">
         <v>0.62180000000000002</v>
@@ -2786,12 +2773,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" s="13">
         <v>21.979706</v>
@@ -2890,12 +2877,12 @@
         <v>-2.72E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C32" s="13">
         <v>3.1476000000000002</v>
@@ -2994,12 +2981,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C33" s="13">
         <v>0.97719999999999996</v>
@@ -3098,12 +3085,12 @@
         <v>6.7999999999999999E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="15">
         <v>28.614205999999999</v>
@@ -3202,20 +3189,20 @@
         <v>-3.3E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D37" s="13">
         <v>0</v>
@@ -3308,18 +3295,18 @@
         <v>0</v>
       </c>
       <c r="AH37" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D38" s="13">
         <v>0</v>
@@ -3412,18 +3399,18 @@
         <v>0</v>
       </c>
       <c r="AH38" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D39" s="13">
         <v>3.3792</v>
@@ -3516,18 +3503,18 @@
         <v>17.000202000000002</v>
       </c>
       <c r="AH39" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D40" s="13">
         <v>3.2778</v>
@@ -3620,18 +3607,18 @@
         <v>4.5458990000000004</v>
       </c>
       <c r="AH40" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" s="13">
         <v>1.1000000000000001</v>
@@ -3724,18 +3711,18 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AH41" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D42" s="13">
         <v>0</v>
@@ -3828,18 +3815,18 @@
         <v>0</v>
       </c>
       <c r="AH42" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" s="13">
         <v>3.7745000000000002</v>
@@ -3932,18 +3919,18 @@
         <v>12.9628</v>
       </c>
       <c r="AH43" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D44" s="13">
         <v>2.6100000000000002E-2</v>
@@ -4036,18 +4023,18 @@
         <v>2.6100000000000002E-2</v>
       </c>
       <c r="AH44" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="D45" s="13">
         <v>19.650895999999999</v>
@@ -4140,18 +4127,18 @@
         <v>55.921703000000001</v>
       </c>
       <c r="AH45" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D46" s="13">
         <v>0</v>
@@ -4244,18 +4231,18 @@
         <v>0</v>
       </c>
       <c r="AH46" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D47" s="15">
         <v>31.208511000000001</v>
@@ -4348,23 +4335,23 @@
         <v>92.656730999999994</v>
       </c>
       <c r="AH47" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B48" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D49" s="13">
         <v>0</v>
@@ -4457,18 +4444,18 @@
         <v>0</v>
       </c>
       <c r="AH49" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D50" s="13">
         <v>0</v>
@@ -4561,18 +4548,18 @@
         <v>0</v>
       </c>
       <c r="AH50" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D51" s="13">
         <v>0</v>
@@ -4665,18 +4652,18 @@
         <v>219.86515800000001</v>
       </c>
       <c r="AH51" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52" s="13">
         <v>8.7081459999999993</v>
@@ -4769,18 +4756,18 @@
         <v>170.64920000000001</v>
       </c>
       <c r="AH52" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D53" s="13">
         <v>0</v>
@@ -4873,18 +4860,18 @@
         <v>0</v>
       </c>
       <c r="AH53" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D54" s="13">
         <v>0</v>
@@ -4977,18 +4964,18 @@
         <v>0</v>
       </c>
       <c r="AH54" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D55" s="13">
         <v>0</v>
@@ -5081,18 +5068,18 @@
         <v>1.666782</v>
       </c>
       <c r="AH55" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D56" s="13">
         <v>0</v>
@@ -5185,18 +5172,18 @@
         <v>4.2449999999999996E-3</v>
       </c>
       <c r="AH56" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="D57" s="13">
         <v>0.100994</v>
@@ -5289,18 +5276,18 @@
         <v>317.91125499999998</v>
       </c>
       <c r="AH57" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D58" s="13">
         <v>0</v>
@@ -5393,18 +5380,18 @@
         <v>36.505851999999997</v>
       </c>
       <c r="AH58" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D59" s="15">
         <v>8.8091390000000001</v>
@@ -5497,18 +5484,18 @@
         <v>746.60253899999998</v>
       </c>
       <c r="AH59" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D60" s="15">
         <v>40.017651000000001</v>
@@ -5601,23 +5588,23 @@
         <v>839.259277</v>
       </c>
       <c r="AH60" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D63" s="13">
         <v>4.5084</v>
@@ -5710,18 +5697,18 @@
         <v>128.09979200000001</v>
       </c>
       <c r="AH63" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D64" s="13">
         <v>1.1951000000000001</v>
@@ -5814,18 +5801,18 @@
         <v>37.574706999999997</v>
       </c>
       <c r="AH64" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D65" s="13">
         <v>5.6000000000000001E-2</v>
@@ -5918,18 +5905,18 @@
         <v>9.9011019999999998</v>
       </c>
       <c r="AH65" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D66" s="13">
         <v>1.8800000000000001E-2</v>
@@ -6022,18 +6009,18 @@
         <v>4.3529010000000001</v>
       </c>
       <c r="AH66" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D67" s="13">
         <v>5.7363</v>
@@ -6126,18 +6113,18 @@
         <v>59.417895999999999</v>
       </c>
       <c r="AH67" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D68" s="13">
         <v>0</v>
@@ -6230,18 +6217,18 @@
         <v>0</v>
       </c>
       <c r="AH68" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D69" s="13">
         <v>0</v>
@@ -6334,18 +6321,18 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AH69" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D70" s="13">
         <v>0</v>
@@ -6438,18 +6425,18 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="AH70" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B71" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="D71" s="13">
         <v>0</v>
@@ -6542,18 +6529,18 @@
         <v>0.40960000000000002</v>
       </c>
       <c r="AH71" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D72" s="15">
         <v>11.514602999999999</v>
@@ -6646,15 +6633,15 @@
         <v>239.796066</v>
       </c>
       <c r="AH72" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C74" s="15">
         <v>1091.1827390000001</v>
@@ -6753,17 +6740,17 @@
         <v>1.4742999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C77" s="13">
         <v>1.94556</v>
@@ -6862,12 +6849,12 @@
         <v>-1.4040000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C78" s="13">
         <v>0.56876099999999996</v>
@@ -6966,12 +6953,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C79" s="13">
         <v>17.840422</v>
@@ -7070,12 +7057,12 @@
         <v>2.2790999999999999E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C80" s="13">
         <v>2.8463500000000002</v>
@@ -7174,12 +7161,12 @@
         <v>5.0600000000000005E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C81" s="13">
         <v>40.204830000000001</v>
@@ -7278,12 +7265,12 @@
         <v>4.8174000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C82" s="13">
         <v>0.63580000000000003</v>
@@ -7382,12 +7369,12 @@
         <v>2.5270000000000002E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C83" s="15">
         <v>64.041725</v>
@@ -7486,15 +7473,15 @@
         <v>3.9715E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D85" s="15">
         <v>6.1937160000000002</v>
@@ -7587,890 +7574,890 @@
         <v>142.10734600000001</v>
       </c>
       <c r="AH85" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="28"/>
+      <c r="J87" s="28"/>
+      <c r="K87" s="28"/>
+      <c r="L87" s="28"/>
+      <c r="M87" s="28"/>
+      <c r="N87" s="28"/>
+      <c r="O87" s="28"/>
+      <c r="P87" s="28"/>
+      <c r="Q87" s="28"/>
+      <c r="R87" s="28"/>
+      <c r="S87" s="28"/>
+      <c r="T87" s="28"/>
+      <c r="U87" s="28"/>
+      <c r="V87" s="28"/>
+      <c r="W87" s="28"/>
+      <c r="X87" s="28"/>
+      <c r="Y87" s="28"/>
+      <c r="Z87" s="28"/>
+      <c r="AA87" s="28"/>
+      <c r="AB87" s="28"/>
+      <c r="AC87" s="28"/>
+      <c r="AD87" s="28"/>
+      <c r="AE87" s="28"/>
+      <c r="AF87" s="28"/>
+      <c r="AG87" s="28"/>
+      <c r="AH87" s="21"/>
+    </row>
+    <row r="88" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="29"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
-      <c r="L87" s="29"/>
-      <c r="M87" s="29"/>
-      <c r="N87" s="29"/>
-      <c r="O87" s="29"/>
-      <c r="P87" s="29"/>
-      <c r="Q87" s="29"/>
-      <c r="R87" s="29"/>
-      <c r="S87" s="29"/>
-      <c r="T87" s="29"/>
-      <c r="U87" s="29"/>
-      <c r="V87" s="29"/>
-      <c r="W87" s="29"/>
-      <c r="X87" s="29"/>
-      <c r="Y87" s="29"/>
-      <c r="Z87" s="29"/>
-      <c r="AA87" s="29"/>
-      <c r="AB87" s="29"/>
-      <c r="AC87" s="29"/>
-      <c r="AD87" s="29"/>
-      <c r="AE87" s="29"/>
-      <c r="AF87" s="29"/>
-      <c r="AG87" s="29"/>
-      <c r="AH87" s="21"/>
-    </row>
-    <row r="88" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="7" t="s">
+    </row>
+    <row r="91" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="B92" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="97" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="89" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="90" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="91" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B92" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="95" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="96" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="7" t="s">
+    <row r="101" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B101" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B102" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="103" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="104" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="99" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="7" t="s">
+    <row r="105" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B101" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="102" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B102" s="7" t="s">
+    <row r="106" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="103" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="7" t="s">
+    <row r="107" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="104" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="105" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="7" t="s">
+    <row r="108" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="107" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="7" t="s">
+    <row r="109" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="108" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="7" t="s">
+    <row r="110" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="7" t="s">
+    <row r="111" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="111" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="112" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="27"/>
-      <c r="M112" s="27"/>
-      <c r="N112" s="27"/>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
-      <c r="Q112" s="27"/>
-      <c r="R112" s="27"/>
-      <c r="S112" s="27"/>
-      <c r="T112" s="27"/>
-      <c r="U112" s="27"/>
-      <c r="V112" s="27"/>
-      <c r="W112" s="27"/>
-      <c r="X112" s="27"/>
-      <c r="Y112" s="27"/>
-      <c r="Z112" s="27"/>
-      <c r="AA112" s="27"/>
-      <c r="AB112" s="27"/>
-      <c r="AC112" s="27"/>
-      <c r="AD112" s="27"/>
-      <c r="AE112" s="27"/>
-      <c r="AF112" s="27"/>
-      <c r="AG112" s="27"/>
-      <c r="AH112" s="27"/>
-    </row>
-    <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="27"/>
-      <c r="C308" s="27"/>
-      <c r="D308" s="27"/>
-      <c r="E308" s="27"/>
-      <c r="F308" s="27"/>
-      <c r="G308" s="27"/>
-      <c r="H308" s="27"/>
-      <c r="I308" s="27"/>
-      <c r="J308" s="27"/>
-      <c r="K308" s="27"/>
-      <c r="L308" s="27"/>
-      <c r="M308" s="27"/>
-      <c r="N308" s="27"/>
-      <c r="O308" s="27"/>
-      <c r="P308" s="27"/>
-      <c r="Q308" s="27"/>
-      <c r="R308" s="27"/>
-      <c r="S308" s="27"/>
-      <c r="T308" s="27"/>
-      <c r="U308" s="27"/>
-      <c r="V308" s="27"/>
-      <c r="W308" s="27"/>
-      <c r="X308" s="27"/>
-      <c r="Y308" s="27"/>
-      <c r="Z308" s="27"/>
-      <c r="AA308" s="27"/>
-      <c r="AB308" s="27"/>
-      <c r="AC308" s="27"/>
-      <c r="AD308" s="27"/>
-      <c r="AE308" s="27"/>
-      <c r="AF308" s="27"/>
-      <c r="AG308" s="27"/>
-      <c r="AH308" s="27"/>
-    </row>
-    <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B511" s="27"/>
-      <c r="C511" s="27"/>
-      <c r="D511" s="27"/>
-      <c r="E511" s="27"/>
-      <c r="F511" s="27"/>
-      <c r="G511" s="27"/>
-      <c r="H511" s="27"/>
-      <c r="I511" s="27"/>
-      <c r="J511" s="27"/>
-      <c r="K511" s="27"/>
-      <c r="L511" s="27"/>
-      <c r="M511" s="27"/>
-      <c r="N511" s="27"/>
-      <c r="O511" s="27"/>
-      <c r="P511" s="27"/>
-      <c r="Q511" s="27"/>
-      <c r="R511" s="27"/>
-      <c r="S511" s="27"/>
-      <c r="T511" s="27"/>
-      <c r="U511" s="27"/>
-      <c r="V511" s="27"/>
-      <c r="W511" s="27"/>
-      <c r="X511" s="27"/>
-      <c r="Y511" s="27"/>
-      <c r="Z511" s="27"/>
-      <c r="AA511" s="27"/>
-      <c r="AB511" s="27"/>
-      <c r="AC511" s="27"/>
-      <c r="AD511" s="27"/>
-      <c r="AE511" s="27"/>
-      <c r="AF511" s="27"/>
-      <c r="AG511" s="27"/>
-      <c r="AH511" s="27"/>
-    </row>
-    <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="27"/>
-      <c r="C712" s="27"/>
-      <c r="D712" s="27"/>
-      <c r="E712" s="27"/>
-      <c r="F712" s="27"/>
-      <c r="G712" s="27"/>
-      <c r="H712" s="27"/>
-      <c r="I712" s="27"/>
-      <c r="J712" s="27"/>
-      <c r="K712" s="27"/>
-      <c r="L712" s="27"/>
-      <c r="M712" s="27"/>
-      <c r="N712" s="27"/>
-      <c r="O712" s="27"/>
-      <c r="P712" s="27"/>
-      <c r="Q712" s="27"/>
-      <c r="R712" s="27"/>
-      <c r="S712" s="27"/>
-      <c r="T712" s="27"/>
-      <c r="U712" s="27"/>
-      <c r="V712" s="27"/>
-      <c r="W712" s="27"/>
-      <c r="X712" s="27"/>
-      <c r="Y712" s="27"/>
-      <c r="Z712" s="27"/>
-      <c r="AA712" s="27"/>
-      <c r="AB712" s="27"/>
-      <c r="AC712" s="27"/>
-      <c r="AD712" s="27"/>
-      <c r="AE712" s="27"/>
-      <c r="AF712" s="27"/>
-      <c r="AG712" s="27"/>
-      <c r="AH712" s="27"/>
-    </row>
-    <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B887" s="27"/>
-      <c r="C887" s="27"/>
-      <c r="D887" s="27"/>
-      <c r="E887" s="27"/>
-      <c r="F887" s="27"/>
-      <c r="G887" s="27"/>
-      <c r="H887" s="27"/>
-      <c r="I887" s="27"/>
-      <c r="J887" s="27"/>
-      <c r="K887" s="27"/>
-      <c r="L887" s="27"/>
-      <c r="M887" s="27"/>
-      <c r="N887" s="27"/>
-      <c r="O887" s="27"/>
-      <c r="P887" s="27"/>
-      <c r="Q887" s="27"/>
-      <c r="R887" s="27"/>
-      <c r="S887" s="27"/>
-      <c r="T887" s="27"/>
-      <c r="U887" s="27"/>
-      <c r="V887" s="27"/>
-      <c r="W887" s="27"/>
-      <c r="X887" s="27"/>
-      <c r="Y887" s="27"/>
-      <c r="Z887" s="27"/>
-      <c r="AA887" s="27"/>
-      <c r="AB887" s="27"/>
-      <c r="AC887" s="27"/>
-      <c r="AD887" s="27"/>
-      <c r="AE887" s="27"/>
-      <c r="AF887" s="27"/>
-      <c r="AG887" s="27"/>
-      <c r="AH887" s="27"/>
-    </row>
-    <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="27"/>
-      <c r="C1100" s="27"/>
-      <c r="D1100" s="27"/>
-      <c r="E1100" s="27"/>
-      <c r="F1100" s="27"/>
-      <c r="G1100" s="27"/>
-      <c r="H1100" s="27"/>
-      <c r="I1100" s="27"/>
-      <c r="J1100" s="27"/>
-      <c r="K1100" s="27"/>
-      <c r="L1100" s="27"/>
-      <c r="M1100" s="27"/>
-      <c r="N1100" s="27"/>
-      <c r="O1100" s="27"/>
-      <c r="P1100" s="27"/>
-      <c r="Q1100" s="27"/>
-      <c r="R1100" s="27"/>
-      <c r="S1100" s="27"/>
-      <c r="T1100" s="27"/>
-      <c r="U1100" s="27"/>
-      <c r="V1100" s="27"/>
-      <c r="W1100" s="27"/>
-      <c r="X1100" s="27"/>
-      <c r="Y1100" s="27"/>
-      <c r="Z1100" s="27"/>
-      <c r="AA1100" s="27"/>
-      <c r="AB1100" s="27"/>
-      <c r="AC1100" s="27"/>
-      <c r="AD1100" s="27"/>
-      <c r="AE1100" s="27"/>
-      <c r="AF1100" s="27"/>
-      <c r="AG1100" s="27"/>
-      <c r="AH1100" s="27"/>
-    </row>
-    <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1227" s="27"/>
-      <c r="C1227" s="27"/>
-      <c r="D1227" s="27"/>
-      <c r="E1227" s="27"/>
-      <c r="F1227" s="27"/>
-      <c r="G1227" s="27"/>
-      <c r="H1227" s="27"/>
-      <c r="I1227" s="27"/>
-      <c r="J1227" s="27"/>
-      <c r="K1227" s="27"/>
-      <c r="L1227" s="27"/>
-      <c r="M1227" s="27"/>
-      <c r="N1227" s="27"/>
-      <c r="O1227" s="27"/>
-      <c r="P1227" s="27"/>
-      <c r="Q1227" s="27"/>
-      <c r="R1227" s="27"/>
-      <c r="S1227" s="27"/>
-      <c r="T1227" s="27"/>
-      <c r="U1227" s="27"/>
-      <c r="V1227" s="27"/>
-      <c r="W1227" s="27"/>
-      <c r="X1227" s="27"/>
-      <c r="Y1227" s="27"/>
-      <c r="Z1227" s="27"/>
-      <c r="AA1227" s="27"/>
-      <c r="AB1227" s="27"/>
-      <c r="AC1227" s="27"/>
-      <c r="AD1227" s="27"/>
-      <c r="AE1227" s="27"/>
-      <c r="AF1227" s="27"/>
-      <c r="AG1227" s="27"/>
-      <c r="AH1227" s="27"/>
-    </row>
-    <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1390" s="27"/>
-      <c r="C1390" s="27"/>
-      <c r="D1390" s="27"/>
-      <c r="E1390" s="27"/>
-      <c r="F1390" s="27"/>
-      <c r="G1390" s="27"/>
-      <c r="H1390" s="27"/>
-      <c r="I1390" s="27"/>
-      <c r="J1390" s="27"/>
-      <c r="K1390" s="27"/>
-      <c r="L1390" s="27"/>
-      <c r="M1390" s="27"/>
-      <c r="N1390" s="27"/>
-      <c r="O1390" s="27"/>
-      <c r="P1390" s="27"/>
-      <c r="Q1390" s="27"/>
-      <c r="R1390" s="27"/>
-      <c r="S1390" s="27"/>
-      <c r="T1390" s="27"/>
-      <c r="U1390" s="27"/>
-      <c r="V1390" s="27"/>
-      <c r="W1390" s="27"/>
-      <c r="X1390" s="27"/>
-      <c r="Y1390" s="27"/>
-      <c r="Z1390" s="27"/>
-      <c r="AA1390" s="27"/>
-      <c r="AB1390" s="27"/>
-      <c r="AC1390" s="27"/>
-      <c r="AD1390" s="27"/>
-      <c r="AE1390" s="27"/>
-      <c r="AF1390" s="27"/>
-      <c r="AG1390" s="27"/>
-      <c r="AH1390" s="27"/>
-    </row>
-    <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1502" s="27"/>
-      <c r="C1502" s="27"/>
-      <c r="D1502" s="27"/>
-      <c r="E1502" s="27"/>
-      <c r="F1502" s="27"/>
-      <c r="G1502" s="27"/>
-      <c r="H1502" s="27"/>
-      <c r="I1502" s="27"/>
-      <c r="J1502" s="27"/>
-      <c r="K1502" s="27"/>
-      <c r="L1502" s="27"/>
-      <c r="M1502" s="27"/>
-      <c r="N1502" s="27"/>
-      <c r="O1502" s="27"/>
-      <c r="P1502" s="27"/>
-      <c r="Q1502" s="27"/>
-      <c r="R1502" s="27"/>
-      <c r="S1502" s="27"/>
-      <c r="T1502" s="27"/>
-      <c r="U1502" s="27"/>
-      <c r="V1502" s="27"/>
-      <c r="W1502" s="27"/>
-      <c r="X1502" s="27"/>
-      <c r="Y1502" s="27"/>
-      <c r="Z1502" s="27"/>
-      <c r="AA1502" s="27"/>
-      <c r="AB1502" s="27"/>
-      <c r="AC1502" s="27"/>
-      <c r="AD1502" s="27"/>
-      <c r="AE1502" s="27"/>
-      <c r="AF1502" s="27"/>
-      <c r="AG1502" s="27"/>
-      <c r="AH1502" s="27"/>
-    </row>
-    <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1604" s="27"/>
-      <c r="C1604" s="27"/>
-      <c r="D1604" s="27"/>
-      <c r="E1604" s="27"/>
-      <c r="F1604" s="27"/>
-      <c r="G1604" s="27"/>
-      <c r="H1604" s="27"/>
-      <c r="I1604" s="27"/>
-      <c r="J1604" s="27"/>
-      <c r="K1604" s="27"/>
-      <c r="L1604" s="27"/>
-      <c r="M1604" s="27"/>
-      <c r="N1604" s="27"/>
-      <c r="O1604" s="27"/>
-      <c r="P1604" s="27"/>
-      <c r="Q1604" s="27"/>
-      <c r="R1604" s="27"/>
-      <c r="S1604" s="27"/>
-      <c r="T1604" s="27"/>
-      <c r="U1604" s="27"/>
-      <c r="V1604" s="27"/>
-      <c r="W1604" s="27"/>
-      <c r="X1604" s="27"/>
-      <c r="Y1604" s="27"/>
-      <c r="Z1604" s="27"/>
-      <c r="AA1604" s="27"/>
-      <c r="AB1604" s="27"/>
-      <c r="AC1604" s="27"/>
-      <c r="AD1604" s="27"/>
-      <c r="AE1604" s="27"/>
-      <c r="AF1604" s="27"/>
-      <c r="AG1604" s="27"/>
-      <c r="AH1604" s="27"/>
-    </row>
-    <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1698" s="27"/>
-      <c r="C1698" s="27"/>
-      <c r="D1698" s="27"/>
-      <c r="E1698" s="27"/>
-      <c r="F1698" s="27"/>
-      <c r="G1698" s="27"/>
-      <c r="H1698" s="27"/>
-      <c r="I1698" s="27"/>
-      <c r="J1698" s="27"/>
-      <c r="K1698" s="27"/>
-      <c r="L1698" s="27"/>
-      <c r="M1698" s="27"/>
-      <c r="N1698" s="27"/>
-      <c r="O1698" s="27"/>
-      <c r="P1698" s="27"/>
-      <c r="Q1698" s="27"/>
-      <c r="R1698" s="27"/>
-      <c r="S1698" s="27"/>
-      <c r="T1698" s="27"/>
-      <c r="U1698" s="27"/>
-      <c r="V1698" s="27"/>
-      <c r="W1698" s="27"/>
-      <c r="X1698" s="27"/>
-      <c r="Y1698" s="27"/>
-      <c r="Z1698" s="27"/>
-      <c r="AA1698" s="27"/>
-      <c r="AB1698" s="27"/>
-      <c r="AC1698" s="27"/>
-      <c r="AD1698" s="27"/>
-      <c r="AE1698" s="27"/>
-      <c r="AF1698" s="27"/>
-      <c r="AG1698" s="27"/>
-      <c r="AH1698" s="27"/>
-    </row>
-    <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1945" s="27"/>
-      <c r="C1945" s="27"/>
-      <c r="D1945" s="27"/>
-      <c r="E1945" s="27"/>
-      <c r="F1945" s="27"/>
-      <c r="G1945" s="27"/>
-      <c r="H1945" s="27"/>
-      <c r="I1945" s="27"/>
-      <c r="J1945" s="27"/>
-      <c r="K1945" s="27"/>
-      <c r="L1945" s="27"/>
-      <c r="M1945" s="27"/>
-      <c r="N1945" s="27"/>
-      <c r="O1945" s="27"/>
-      <c r="P1945" s="27"/>
-      <c r="Q1945" s="27"/>
-      <c r="R1945" s="27"/>
-      <c r="S1945" s="27"/>
-      <c r="T1945" s="27"/>
-      <c r="U1945" s="27"/>
-      <c r="V1945" s="27"/>
-      <c r="W1945" s="27"/>
-      <c r="X1945" s="27"/>
-      <c r="Y1945" s="27"/>
-      <c r="Z1945" s="27"/>
-      <c r="AA1945" s="27"/>
-      <c r="AB1945" s="27"/>
-      <c r="AC1945" s="27"/>
-      <c r="AD1945" s="27"/>
-      <c r="AE1945" s="27"/>
-      <c r="AF1945" s="27"/>
-      <c r="AG1945" s="27"/>
-      <c r="AH1945" s="27"/>
-    </row>
-    <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2031" s="27"/>
-      <c r="C2031" s="27"/>
-      <c r="D2031" s="27"/>
-      <c r="E2031" s="27"/>
-      <c r="F2031" s="27"/>
-      <c r="G2031" s="27"/>
-      <c r="H2031" s="27"/>
-      <c r="I2031" s="27"/>
-      <c r="J2031" s="27"/>
-      <c r="K2031" s="27"/>
-      <c r="L2031" s="27"/>
-      <c r="M2031" s="27"/>
-      <c r="N2031" s="27"/>
-      <c r="O2031" s="27"/>
-      <c r="P2031" s="27"/>
-      <c r="Q2031" s="27"/>
-      <c r="R2031" s="27"/>
-      <c r="S2031" s="27"/>
-      <c r="T2031" s="27"/>
-      <c r="U2031" s="27"/>
-      <c r="V2031" s="27"/>
-      <c r="W2031" s="27"/>
-      <c r="X2031" s="27"/>
-      <c r="Y2031" s="27"/>
-      <c r="Z2031" s="27"/>
-      <c r="AA2031" s="27"/>
-      <c r="AB2031" s="27"/>
-      <c r="AC2031" s="27"/>
-      <c r="AD2031" s="27"/>
-      <c r="AE2031" s="27"/>
-      <c r="AF2031" s="27"/>
-      <c r="AG2031" s="27"/>
-      <c r="AH2031" s="27"/>
-    </row>
-    <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2153" s="27"/>
-      <c r="C2153" s="27"/>
-      <c r="D2153" s="27"/>
-      <c r="E2153" s="27"/>
-      <c r="F2153" s="27"/>
-      <c r="G2153" s="27"/>
-      <c r="H2153" s="27"/>
-      <c r="I2153" s="27"/>
-      <c r="J2153" s="27"/>
-      <c r="K2153" s="27"/>
-      <c r="L2153" s="27"/>
-      <c r="M2153" s="27"/>
-      <c r="N2153" s="27"/>
-      <c r="O2153" s="27"/>
-      <c r="P2153" s="27"/>
-      <c r="Q2153" s="27"/>
-      <c r="R2153" s="27"/>
-      <c r="S2153" s="27"/>
-      <c r="T2153" s="27"/>
-      <c r="U2153" s="27"/>
-      <c r="V2153" s="27"/>
-      <c r="W2153" s="27"/>
-      <c r="X2153" s="27"/>
-      <c r="Y2153" s="27"/>
-      <c r="Z2153" s="27"/>
-      <c r="AA2153" s="27"/>
-      <c r="AB2153" s="27"/>
-      <c r="AC2153" s="27"/>
-      <c r="AD2153" s="27"/>
-      <c r="AE2153" s="27"/>
-      <c r="AF2153" s="27"/>
-      <c r="AG2153" s="27"/>
-      <c r="AH2153" s="27"/>
-    </row>
-    <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2317" s="27"/>
-      <c r="C2317" s="27"/>
-      <c r="D2317" s="27"/>
-      <c r="E2317" s="27"/>
-      <c r="F2317" s="27"/>
-      <c r="G2317" s="27"/>
-      <c r="H2317" s="27"/>
-      <c r="I2317" s="27"/>
-      <c r="J2317" s="27"/>
-      <c r="K2317" s="27"/>
-      <c r="L2317" s="27"/>
-      <c r="M2317" s="27"/>
-      <c r="N2317" s="27"/>
-      <c r="O2317" s="27"/>
-      <c r="P2317" s="27"/>
-      <c r="Q2317" s="27"/>
-      <c r="R2317" s="27"/>
-      <c r="S2317" s="27"/>
-      <c r="T2317" s="27"/>
-      <c r="U2317" s="27"/>
-      <c r="V2317" s="27"/>
-      <c r="W2317" s="27"/>
-      <c r="X2317" s="27"/>
-      <c r="Y2317" s="27"/>
-      <c r="Z2317" s="27"/>
-      <c r="AA2317" s="27"/>
-      <c r="AB2317" s="27"/>
-      <c r="AC2317" s="27"/>
-      <c r="AD2317" s="27"/>
-      <c r="AE2317" s="27"/>
-      <c r="AF2317" s="27"/>
-      <c r="AG2317" s="27"/>
-      <c r="AH2317" s="27"/>
-    </row>
-    <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2419" s="27"/>
-      <c r="C2419" s="27"/>
-      <c r="D2419" s="27"/>
-      <c r="E2419" s="27"/>
-      <c r="F2419" s="27"/>
-      <c r="G2419" s="27"/>
-      <c r="H2419" s="27"/>
-      <c r="I2419" s="27"/>
-      <c r="J2419" s="27"/>
-      <c r="K2419" s="27"/>
-      <c r="L2419" s="27"/>
-      <c r="M2419" s="27"/>
-      <c r="N2419" s="27"/>
-      <c r="O2419" s="27"/>
-      <c r="P2419" s="27"/>
-      <c r="Q2419" s="27"/>
-      <c r="R2419" s="27"/>
-      <c r="S2419" s="27"/>
-      <c r="T2419" s="27"/>
-      <c r="U2419" s="27"/>
-      <c r="V2419" s="27"/>
-      <c r="W2419" s="27"/>
-      <c r="X2419" s="27"/>
-      <c r="Y2419" s="27"/>
-      <c r="Z2419" s="27"/>
-      <c r="AA2419" s="27"/>
-      <c r="AB2419" s="27"/>
-      <c r="AC2419" s="27"/>
-      <c r="AD2419" s="27"/>
-      <c r="AE2419" s="27"/>
-      <c r="AF2419" s="27"/>
-      <c r="AG2419" s="27"/>
-      <c r="AH2419" s="27"/>
-    </row>
-    <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2509" s="27"/>
-      <c r="C2509" s="27"/>
-      <c r="D2509" s="27"/>
-      <c r="E2509" s="27"/>
-      <c r="F2509" s="27"/>
-      <c r="G2509" s="27"/>
-      <c r="H2509" s="27"/>
-      <c r="I2509" s="27"/>
-      <c r="J2509" s="27"/>
-      <c r="K2509" s="27"/>
-      <c r="L2509" s="27"/>
-      <c r="M2509" s="27"/>
-      <c r="N2509" s="27"/>
-      <c r="O2509" s="27"/>
-      <c r="P2509" s="27"/>
-      <c r="Q2509" s="27"/>
-      <c r="R2509" s="27"/>
-      <c r="S2509" s="27"/>
-      <c r="T2509" s="27"/>
-      <c r="U2509" s="27"/>
-      <c r="V2509" s="27"/>
-      <c r="W2509" s="27"/>
-      <c r="X2509" s="27"/>
-      <c r="Y2509" s="27"/>
-      <c r="Z2509" s="27"/>
-      <c r="AA2509" s="27"/>
-      <c r="AB2509" s="27"/>
-      <c r="AC2509" s="27"/>
-      <c r="AD2509" s="27"/>
-      <c r="AE2509" s="27"/>
-      <c r="AF2509" s="27"/>
-      <c r="AG2509" s="27"/>
-      <c r="AH2509" s="27"/>
-    </row>
-    <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2598" s="27"/>
-      <c r="C2598" s="27"/>
-      <c r="D2598" s="27"/>
-      <c r="E2598" s="27"/>
-      <c r="F2598" s="27"/>
-      <c r="G2598" s="27"/>
-      <c r="H2598" s="27"/>
-      <c r="I2598" s="27"/>
-      <c r="J2598" s="27"/>
-      <c r="K2598" s="27"/>
-      <c r="L2598" s="27"/>
-      <c r="M2598" s="27"/>
-      <c r="N2598" s="27"/>
-      <c r="O2598" s="27"/>
-      <c r="P2598" s="27"/>
-      <c r="Q2598" s="27"/>
-      <c r="R2598" s="27"/>
-      <c r="S2598" s="27"/>
-      <c r="T2598" s="27"/>
-      <c r="U2598" s="27"/>
-      <c r="V2598" s="27"/>
-      <c r="W2598" s="27"/>
-      <c r="X2598" s="27"/>
-      <c r="Y2598" s="27"/>
-      <c r="Z2598" s="27"/>
-      <c r="AA2598" s="27"/>
-      <c r="AB2598" s="27"/>
-      <c r="AC2598" s="27"/>
-      <c r="AD2598" s="27"/>
-      <c r="AE2598" s="27"/>
-      <c r="AF2598" s="27"/>
-      <c r="AG2598" s="27"/>
-      <c r="AH2598" s="27"/>
-    </row>
-    <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2719" s="27"/>
-      <c r="C2719" s="27"/>
-      <c r="D2719" s="27"/>
-      <c r="E2719" s="27"/>
-      <c r="F2719" s="27"/>
-      <c r="G2719" s="27"/>
-      <c r="H2719" s="27"/>
-      <c r="I2719" s="27"/>
-      <c r="J2719" s="27"/>
-      <c r="K2719" s="27"/>
-      <c r="L2719" s="27"/>
-      <c r="M2719" s="27"/>
-      <c r="N2719" s="27"/>
-      <c r="O2719" s="27"/>
-      <c r="P2719" s="27"/>
-      <c r="Q2719" s="27"/>
-      <c r="R2719" s="27"/>
-      <c r="S2719" s="27"/>
-      <c r="T2719" s="27"/>
-      <c r="U2719" s="27"/>
-      <c r="V2719" s="27"/>
-      <c r="W2719" s="27"/>
-      <c r="X2719" s="27"/>
-      <c r="Y2719" s="27"/>
-      <c r="Z2719" s="27"/>
-      <c r="AA2719" s="27"/>
-      <c r="AB2719" s="27"/>
-      <c r="AC2719" s="27"/>
-      <c r="AD2719" s="27"/>
-      <c r="AE2719" s="27"/>
-      <c r="AF2719" s="27"/>
-      <c r="AG2719" s="27"/>
-      <c r="AH2719" s="27"/>
-    </row>
-    <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2837" s="27"/>
-      <c r="C2837" s="27"/>
-      <c r="D2837" s="27"/>
-      <c r="E2837" s="27"/>
-      <c r="F2837" s="27"/>
-      <c r="G2837" s="27"/>
-      <c r="H2837" s="27"/>
-      <c r="I2837" s="27"/>
-      <c r="J2837" s="27"/>
-      <c r="K2837" s="27"/>
-      <c r="L2837" s="27"/>
-      <c r="M2837" s="27"/>
-      <c r="N2837" s="27"/>
-      <c r="O2837" s="27"/>
-      <c r="P2837" s="27"/>
-      <c r="Q2837" s="27"/>
-      <c r="R2837" s="27"/>
-      <c r="S2837" s="27"/>
-      <c r="T2837" s="27"/>
-      <c r="U2837" s="27"/>
-      <c r="V2837" s="27"/>
-      <c r="W2837" s="27"/>
-      <c r="X2837" s="27"/>
-      <c r="Y2837" s="27"/>
-      <c r="Z2837" s="27"/>
-      <c r="AA2837" s="27"/>
-      <c r="AB2837" s="27"/>
-      <c r="AC2837" s="27"/>
-      <c r="AD2837" s="27"/>
-      <c r="AE2837" s="27"/>
-      <c r="AF2837" s="27"/>
-      <c r="AG2837" s="27"/>
-      <c r="AH2837" s="27"/>
+    <row r="112" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="29"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="29"/>
+      <c r="F112" s="29"/>
+      <c r="G112" s="29"/>
+      <c r="H112" s="29"/>
+      <c r="I112" s="29"/>
+      <c r="J112" s="29"/>
+      <c r="K112" s="29"/>
+      <c r="L112" s="29"/>
+      <c r="M112" s="29"/>
+      <c r="N112" s="29"/>
+      <c r="O112" s="29"/>
+      <c r="P112" s="29"/>
+      <c r="Q112" s="29"/>
+      <c r="R112" s="29"/>
+      <c r="S112" s="29"/>
+      <c r="T112" s="29"/>
+      <c r="U112" s="29"/>
+      <c r="V112" s="29"/>
+      <c r="W112" s="29"/>
+      <c r="X112" s="29"/>
+      <c r="Y112" s="29"/>
+      <c r="Z112" s="29"/>
+      <c r="AA112" s="29"/>
+      <c r="AB112" s="29"/>
+      <c r="AC112" s="29"/>
+      <c r="AD112" s="29"/>
+      <c r="AE112" s="29"/>
+      <c r="AF112" s="29"/>
+      <c r="AG112" s="29"/>
+      <c r="AH112" s="29"/>
+    </row>
+    <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B308" s="29"/>
+      <c r="C308" s="29"/>
+      <c r="D308" s="29"/>
+      <c r="E308" s="29"/>
+      <c r="F308" s="29"/>
+      <c r="G308" s="29"/>
+      <c r="H308" s="29"/>
+      <c r="I308" s="29"/>
+      <c r="J308" s="29"/>
+      <c r="K308" s="29"/>
+      <c r="L308" s="29"/>
+      <c r="M308" s="29"/>
+      <c r="N308" s="29"/>
+      <c r="O308" s="29"/>
+      <c r="P308" s="29"/>
+      <c r="Q308" s="29"/>
+      <c r="R308" s="29"/>
+      <c r="S308" s="29"/>
+      <c r="T308" s="29"/>
+      <c r="U308" s="29"/>
+      <c r="V308" s="29"/>
+      <c r="W308" s="29"/>
+      <c r="X308" s="29"/>
+      <c r="Y308" s="29"/>
+      <c r="Z308" s="29"/>
+      <c r="AA308" s="29"/>
+      <c r="AB308" s="29"/>
+      <c r="AC308" s="29"/>
+      <c r="AD308" s="29"/>
+      <c r="AE308" s="29"/>
+      <c r="AF308" s="29"/>
+      <c r="AG308" s="29"/>
+      <c r="AH308" s="29"/>
+    </row>
+    <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B511" s="29"/>
+      <c r="C511" s="29"/>
+      <c r="D511" s="29"/>
+      <c r="E511" s="29"/>
+      <c r="F511" s="29"/>
+      <c r="G511" s="29"/>
+      <c r="H511" s="29"/>
+      <c r="I511" s="29"/>
+      <c r="J511" s="29"/>
+      <c r="K511" s="29"/>
+      <c r="L511" s="29"/>
+      <c r="M511" s="29"/>
+      <c r="N511" s="29"/>
+      <c r="O511" s="29"/>
+      <c r="P511" s="29"/>
+      <c r="Q511" s="29"/>
+      <c r="R511" s="29"/>
+      <c r="S511" s="29"/>
+      <c r="T511" s="29"/>
+      <c r="U511" s="29"/>
+      <c r="V511" s="29"/>
+      <c r="W511" s="29"/>
+      <c r="X511" s="29"/>
+      <c r="Y511" s="29"/>
+      <c r="Z511" s="29"/>
+      <c r="AA511" s="29"/>
+      <c r="AB511" s="29"/>
+      <c r="AC511" s="29"/>
+      <c r="AD511" s="29"/>
+      <c r="AE511" s="29"/>
+      <c r="AF511" s="29"/>
+      <c r="AG511" s="29"/>
+      <c r="AH511" s="29"/>
+    </row>
+    <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B712" s="29"/>
+      <c r="C712" s="29"/>
+      <c r="D712" s="29"/>
+      <c r="E712" s="29"/>
+      <c r="F712" s="29"/>
+      <c r="G712" s="29"/>
+      <c r="H712" s="29"/>
+      <c r="I712" s="29"/>
+      <c r="J712" s="29"/>
+      <c r="K712" s="29"/>
+      <c r="L712" s="29"/>
+      <c r="M712" s="29"/>
+      <c r="N712" s="29"/>
+      <c r="O712" s="29"/>
+      <c r="P712" s="29"/>
+      <c r="Q712" s="29"/>
+      <c r="R712" s="29"/>
+      <c r="S712" s="29"/>
+      <c r="T712" s="29"/>
+      <c r="U712" s="29"/>
+      <c r="V712" s="29"/>
+      <c r="W712" s="29"/>
+      <c r="X712" s="29"/>
+      <c r="Y712" s="29"/>
+      <c r="Z712" s="29"/>
+      <c r="AA712" s="29"/>
+      <c r="AB712" s="29"/>
+      <c r="AC712" s="29"/>
+      <c r="AD712" s="29"/>
+      <c r="AE712" s="29"/>
+      <c r="AF712" s="29"/>
+      <c r="AG712" s="29"/>
+      <c r="AH712" s="29"/>
+    </row>
+    <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B887" s="29"/>
+      <c r="C887" s="29"/>
+      <c r="D887" s="29"/>
+      <c r="E887" s="29"/>
+      <c r="F887" s="29"/>
+      <c r="G887" s="29"/>
+      <c r="H887" s="29"/>
+      <c r="I887" s="29"/>
+      <c r="J887" s="29"/>
+      <c r="K887" s="29"/>
+      <c r="L887" s="29"/>
+      <c r="M887" s="29"/>
+      <c r="N887" s="29"/>
+      <c r="O887" s="29"/>
+      <c r="P887" s="29"/>
+      <c r="Q887" s="29"/>
+      <c r="R887" s="29"/>
+      <c r="S887" s="29"/>
+      <c r="T887" s="29"/>
+      <c r="U887" s="29"/>
+      <c r="V887" s="29"/>
+      <c r="W887" s="29"/>
+      <c r="X887" s="29"/>
+      <c r="Y887" s="29"/>
+      <c r="Z887" s="29"/>
+      <c r="AA887" s="29"/>
+      <c r="AB887" s="29"/>
+      <c r="AC887" s="29"/>
+      <c r="AD887" s="29"/>
+      <c r="AE887" s="29"/>
+      <c r="AF887" s="29"/>
+      <c r="AG887" s="29"/>
+      <c r="AH887" s="29"/>
+    </row>
+    <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1100" s="29"/>
+      <c r="C1100" s="29"/>
+      <c r="D1100" s="29"/>
+      <c r="E1100" s="29"/>
+      <c r="F1100" s="29"/>
+      <c r="G1100" s="29"/>
+      <c r="H1100" s="29"/>
+      <c r="I1100" s="29"/>
+      <c r="J1100" s="29"/>
+      <c r="K1100" s="29"/>
+      <c r="L1100" s="29"/>
+      <c r="M1100" s="29"/>
+      <c r="N1100" s="29"/>
+      <c r="O1100" s="29"/>
+      <c r="P1100" s="29"/>
+      <c r="Q1100" s="29"/>
+      <c r="R1100" s="29"/>
+      <c r="S1100" s="29"/>
+      <c r="T1100" s="29"/>
+      <c r="U1100" s="29"/>
+      <c r="V1100" s="29"/>
+      <c r="W1100" s="29"/>
+      <c r="X1100" s="29"/>
+      <c r="Y1100" s="29"/>
+      <c r="Z1100" s="29"/>
+      <c r="AA1100" s="29"/>
+      <c r="AB1100" s="29"/>
+      <c r="AC1100" s="29"/>
+      <c r="AD1100" s="29"/>
+      <c r="AE1100" s="29"/>
+      <c r="AF1100" s="29"/>
+      <c r="AG1100" s="29"/>
+      <c r="AH1100" s="29"/>
+    </row>
+    <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1227" s="29"/>
+      <c r="C1227" s="29"/>
+      <c r="D1227" s="29"/>
+      <c r="E1227" s="29"/>
+      <c r="F1227" s="29"/>
+      <c r="G1227" s="29"/>
+      <c r="H1227" s="29"/>
+      <c r="I1227" s="29"/>
+      <c r="J1227" s="29"/>
+      <c r="K1227" s="29"/>
+      <c r="L1227" s="29"/>
+      <c r="M1227" s="29"/>
+      <c r="N1227" s="29"/>
+      <c r="O1227" s="29"/>
+      <c r="P1227" s="29"/>
+      <c r="Q1227" s="29"/>
+      <c r="R1227" s="29"/>
+      <c r="S1227" s="29"/>
+      <c r="T1227" s="29"/>
+      <c r="U1227" s="29"/>
+      <c r="V1227" s="29"/>
+      <c r="W1227" s="29"/>
+      <c r="X1227" s="29"/>
+      <c r="Y1227" s="29"/>
+      <c r="Z1227" s="29"/>
+      <c r="AA1227" s="29"/>
+      <c r="AB1227" s="29"/>
+      <c r="AC1227" s="29"/>
+      <c r="AD1227" s="29"/>
+      <c r="AE1227" s="29"/>
+      <c r="AF1227" s="29"/>
+      <c r="AG1227" s="29"/>
+      <c r="AH1227" s="29"/>
+    </row>
+    <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1390" s="29"/>
+      <c r="C1390" s="29"/>
+      <c r="D1390" s="29"/>
+      <c r="E1390" s="29"/>
+      <c r="F1390" s="29"/>
+      <c r="G1390" s="29"/>
+      <c r="H1390" s="29"/>
+      <c r="I1390" s="29"/>
+      <c r="J1390" s="29"/>
+      <c r="K1390" s="29"/>
+      <c r="L1390" s="29"/>
+      <c r="M1390" s="29"/>
+      <c r="N1390" s="29"/>
+      <c r="O1390" s="29"/>
+      <c r="P1390" s="29"/>
+      <c r="Q1390" s="29"/>
+      <c r="R1390" s="29"/>
+      <c r="S1390" s="29"/>
+      <c r="T1390" s="29"/>
+      <c r="U1390" s="29"/>
+      <c r="V1390" s="29"/>
+      <c r="W1390" s="29"/>
+      <c r="X1390" s="29"/>
+      <c r="Y1390" s="29"/>
+      <c r="Z1390" s="29"/>
+      <c r="AA1390" s="29"/>
+      <c r="AB1390" s="29"/>
+      <c r="AC1390" s="29"/>
+      <c r="AD1390" s="29"/>
+      <c r="AE1390" s="29"/>
+      <c r="AF1390" s="29"/>
+      <c r="AG1390" s="29"/>
+      <c r="AH1390" s="29"/>
+    </row>
+    <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1502" s="29"/>
+      <c r="C1502" s="29"/>
+      <c r="D1502" s="29"/>
+      <c r="E1502" s="29"/>
+      <c r="F1502" s="29"/>
+      <c r="G1502" s="29"/>
+      <c r="H1502" s="29"/>
+      <c r="I1502" s="29"/>
+      <c r="J1502" s="29"/>
+      <c r="K1502" s="29"/>
+      <c r="L1502" s="29"/>
+      <c r="M1502" s="29"/>
+      <c r="N1502" s="29"/>
+      <c r="O1502" s="29"/>
+      <c r="P1502" s="29"/>
+      <c r="Q1502" s="29"/>
+      <c r="R1502" s="29"/>
+      <c r="S1502" s="29"/>
+      <c r="T1502" s="29"/>
+      <c r="U1502" s="29"/>
+      <c r="V1502" s="29"/>
+      <c r="W1502" s="29"/>
+      <c r="X1502" s="29"/>
+      <c r="Y1502" s="29"/>
+      <c r="Z1502" s="29"/>
+      <c r="AA1502" s="29"/>
+      <c r="AB1502" s="29"/>
+      <c r="AC1502" s="29"/>
+      <c r="AD1502" s="29"/>
+      <c r="AE1502" s="29"/>
+      <c r="AF1502" s="29"/>
+      <c r="AG1502" s="29"/>
+      <c r="AH1502" s="29"/>
+    </row>
+    <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1604" s="29"/>
+      <c r="C1604" s="29"/>
+      <c r="D1604" s="29"/>
+      <c r="E1604" s="29"/>
+      <c r="F1604" s="29"/>
+      <c r="G1604" s="29"/>
+      <c r="H1604" s="29"/>
+      <c r="I1604" s="29"/>
+      <c r="J1604" s="29"/>
+      <c r="K1604" s="29"/>
+      <c r="L1604" s="29"/>
+      <c r="M1604" s="29"/>
+      <c r="N1604" s="29"/>
+      <c r="O1604" s="29"/>
+      <c r="P1604" s="29"/>
+      <c r="Q1604" s="29"/>
+      <c r="R1604" s="29"/>
+      <c r="S1604" s="29"/>
+      <c r="T1604" s="29"/>
+      <c r="U1604" s="29"/>
+      <c r="V1604" s="29"/>
+      <c r="W1604" s="29"/>
+      <c r="X1604" s="29"/>
+      <c r="Y1604" s="29"/>
+      <c r="Z1604" s="29"/>
+      <c r="AA1604" s="29"/>
+      <c r="AB1604" s="29"/>
+      <c r="AC1604" s="29"/>
+      <c r="AD1604" s="29"/>
+      <c r="AE1604" s="29"/>
+      <c r="AF1604" s="29"/>
+      <c r="AG1604" s="29"/>
+      <c r="AH1604" s="29"/>
+    </row>
+    <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1698" s="29"/>
+      <c r="C1698" s="29"/>
+      <c r="D1698" s="29"/>
+      <c r="E1698" s="29"/>
+      <c r="F1698" s="29"/>
+      <c r="G1698" s="29"/>
+      <c r="H1698" s="29"/>
+      <c r="I1698" s="29"/>
+      <c r="J1698" s="29"/>
+      <c r="K1698" s="29"/>
+      <c r="L1698" s="29"/>
+      <c r="M1698" s="29"/>
+      <c r="N1698" s="29"/>
+      <c r="O1698" s="29"/>
+      <c r="P1698" s="29"/>
+      <c r="Q1698" s="29"/>
+      <c r="R1698" s="29"/>
+      <c r="S1698" s="29"/>
+      <c r="T1698" s="29"/>
+      <c r="U1698" s="29"/>
+      <c r="V1698" s="29"/>
+      <c r="W1698" s="29"/>
+      <c r="X1698" s="29"/>
+      <c r="Y1698" s="29"/>
+      <c r="Z1698" s="29"/>
+      <c r="AA1698" s="29"/>
+      <c r="AB1698" s="29"/>
+      <c r="AC1698" s="29"/>
+      <c r="AD1698" s="29"/>
+      <c r="AE1698" s="29"/>
+      <c r="AF1698" s="29"/>
+      <c r="AG1698" s="29"/>
+      <c r="AH1698" s="29"/>
+    </row>
+    <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1945" s="29"/>
+      <c r="C1945" s="29"/>
+      <c r="D1945" s="29"/>
+      <c r="E1945" s="29"/>
+      <c r="F1945" s="29"/>
+      <c r="G1945" s="29"/>
+      <c r="H1945" s="29"/>
+      <c r="I1945" s="29"/>
+      <c r="J1945" s="29"/>
+      <c r="K1945" s="29"/>
+      <c r="L1945" s="29"/>
+      <c r="M1945" s="29"/>
+      <c r="N1945" s="29"/>
+      <c r="O1945" s="29"/>
+      <c r="P1945" s="29"/>
+      <c r="Q1945" s="29"/>
+      <c r="R1945" s="29"/>
+      <c r="S1945" s="29"/>
+      <c r="T1945" s="29"/>
+      <c r="U1945" s="29"/>
+      <c r="V1945" s="29"/>
+      <c r="W1945" s="29"/>
+      <c r="X1945" s="29"/>
+      <c r="Y1945" s="29"/>
+      <c r="Z1945" s="29"/>
+      <c r="AA1945" s="29"/>
+      <c r="AB1945" s="29"/>
+      <c r="AC1945" s="29"/>
+      <c r="AD1945" s="29"/>
+      <c r="AE1945" s="29"/>
+      <c r="AF1945" s="29"/>
+      <c r="AG1945" s="29"/>
+      <c r="AH1945" s="29"/>
+    </row>
+    <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2031" s="29"/>
+      <c r="C2031" s="29"/>
+      <c r="D2031" s="29"/>
+      <c r="E2031" s="29"/>
+      <c r="F2031" s="29"/>
+      <c r="G2031" s="29"/>
+      <c r="H2031" s="29"/>
+      <c r="I2031" s="29"/>
+      <c r="J2031" s="29"/>
+      <c r="K2031" s="29"/>
+      <c r="L2031" s="29"/>
+      <c r="M2031" s="29"/>
+      <c r="N2031" s="29"/>
+      <c r="O2031" s="29"/>
+      <c r="P2031" s="29"/>
+      <c r="Q2031" s="29"/>
+      <c r="R2031" s="29"/>
+      <c r="S2031" s="29"/>
+      <c r="T2031" s="29"/>
+      <c r="U2031" s="29"/>
+      <c r="V2031" s="29"/>
+      <c r="W2031" s="29"/>
+      <c r="X2031" s="29"/>
+      <c r="Y2031" s="29"/>
+      <c r="Z2031" s="29"/>
+      <c r="AA2031" s="29"/>
+      <c r="AB2031" s="29"/>
+      <c r="AC2031" s="29"/>
+      <c r="AD2031" s="29"/>
+      <c r="AE2031" s="29"/>
+      <c r="AF2031" s="29"/>
+      <c r="AG2031" s="29"/>
+      <c r="AH2031" s="29"/>
+    </row>
+    <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2153" s="29"/>
+      <c r="C2153" s="29"/>
+      <c r="D2153" s="29"/>
+      <c r="E2153" s="29"/>
+      <c r="F2153" s="29"/>
+      <c r="G2153" s="29"/>
+      <c r="H2153" s="29"/>
+      <c r="I2153" s="29"/>
+      <c r="J2153" s="29"/>
+      <c r="K2153" s="29"/>
+      <c r="L2153" s="29"/>
+      <c r="M2153" s="29"/>
+      <c r="N2153" s="29"/>
+      <c r="O2153" s="29"/>
+      <c r="P2153" s="29"/>
+      <c r="Q2153" s="29"/>
+      <c r="R2153" s="29"/>
+      <c r="S2153" s="29"/>
+      <c r="T2153" s="29"/>
+      <c r="U2153" s="29"/>
+      <c r="V2153" s="29"/>
+      <c r="W2153" s="29"/>
+      <c r="X2153" s="29"/>
+      <c r="Y2153" s="29"/>
+      <c r="Z2153" s="29"/>
+      <c r="AA2153" s="29"/>
+      <c r="AB2153" s="29"/>
+      <c r="AC2153" s="29"/>
+      <c r="AD2153" s="29"/>
+      <c r="AE2153" s="29"/>
+      <c r="AF2153" s="29"/>
+      <c r="AG2153" s="29"/>
+      <c r="AH2153" s="29"/>
+    </row>
+    <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2317" s="29"/>
+      <c r="C2317" s="29"/>
+      <c r="D2317" s="29"/>
+      <c r="E2317" s="29"/>
+      <c r="F2317" s="29"/>
+      <c r="G2317" s="29"/>
+      <c r="H2317" s="29"/>
+      <c r="I2317" s="29"/>
+      <c r="J2317" s="29"/>
+      <c r="K2317" s="29"/>
+      <c r="L2317" s="29"/>
+      <c r="M2317" s="29"/>
+      <c r="N2317" s="29"/>
+      <c r="O2317" s="29"/>
+      <c r="P2317" s="29"/>
+      <c r="Q2317" s="29"/>
+      <c r="R2317" s="29"/>
+      <c r="S2317" s="29"/>
+      <c r="T2317" s="29"/>
+      <c r="U2317" s="29"/>
+      <c r="V2317" s="29"/>
+      <c r="W2317" s="29"/>
+      <c r="X2317" s="29"/>
+      <c r="Y2317" s="29"/>
+      <c r="Z2317" s="29"/>
+      <c r="AA2317" s="29"/>
+      <c r="AB2317" s="29"/>
+      <c r="AC2317" s="29"/>
+      <c r="AD2317" s="29"/>
+      <c r="AE2317" s="29"/>
+      <c r="AF2317" s="29"/>
+      <c r="AG2317" s="29"/>
+      <c r="AH2317" s="29"/>
+    </row>
+    <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2419" s="29"/>
+      <c r="C2419" s="29"/>
+      <c r="D2419" s="29"/>
+      <c r="E2419" s="29"/>
+      <c r="F2419" s="29"/>
+      <c r="G2419" s="29"/>
+      <c r="H2419" s="29"/>
+      <c r="I2419" s="29"/>
+      <c r="J2419" s="29"/>
+      <c r="K2419" s="29"/>
+      <c r="L2419" s="29"/>
+      <c r="M2419" s="29"/>
+      <c r="N2419" s="29"/>
+      <c r="O2419" s="29"/>
+      <c r="P2419" s="29"/>
+      <c r="Q2419" s="29"/>
+      <c r="R2419" s="29"/>
+      <c r="S2419" s="29"/>
+      <c r="T2419" s="29"/>
+      <c r="U2419" s="29"/>
+      <c r="V2419" s="29"/>
+      <c r="W2419" s="29"/>
+      <c r="X2419" s="29"/>
+      <c r="Y2419" s="29"/>
+      <c r="Z2419" s="29"/>
+      <c r="AA2419" s="29"/>
+      <c r="AB2419" s="29"/>
+      <c r="AC2419" s="29"/>
+      <c r="AD2419" s="29"/>
+      <c r="AE2419" s="29"/>
+      <c r="AF2419" s="29"/>
+      <c r="AG2419" s="29"/>
+      <c r="AH2419" s="29"/>
+    </row>
+    <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2509" s="29"/>
+      <c r="C2509" s="29"/>
+      <c r="D2509" s="29"/>
+      <c r="E2509" s="29"/>
+      <c r="F2509" s="29"/>
+      <c r="G2509" s="29"/>
+      <c r="H2509" s="29"/>
+      <c r="I2509" s="29"/>
+      <c r="J2509" s="29"/>
+      <c r="K2509" s="29"/>
+      <c r="L2509" s="29"/>
+      <c r="M2509" s="29"/>
+      <c r="N2509" s="29"/>
+      <c r="O2509" s="29"/>
+      <c r="P2509" s="29"/>
+      <c r="Q2509" s="29"/>
+      <c r="R2509" s="29"/>
+      <c r="S2509" s="29"/>
+      <c r="T2509" s="29"/>
+      <c r="U2509" s="29"/>
+      <c r="V2509" s="29"/>
+      <c r="W2509" s="29"/>
+      <c r="X2509" s="29"/>
+      <c r="Y2509" s="29"/>
+      <c r="Z2509" s="29"/>
+      <c r="AA2509" s="29"/>
+      <c r="AB2509" s="29"/>
+      <c r="AC2509" s="29"/>
+      <c r="AD2509" s="29"/>
+      <c r="AE2509" s="29"/>
+      <c r="AF2509" s="29"/>
+      <c r="AG2509" s="29"/>
+      <c r="AH2509" s="29"/>
+    </row>
+    <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2598" s="29"/>
+      <c r="C2598" s="29"/>
+      <c r="D2598" s="29"/>
+      <c r="E2598" s="29"/>
+      <c r="F2598" s="29"/>
+      <c r="G2598" s="29"/>
+      <c r="H2598" s="29"/>
+      <c r="I2598" s="29"/>
+      <c r="J2598" s="29"/>
+      <c r="K2598" s="29"/>
+      <c r="L2598" s="29"/>
+      <c r="M2598" s="29"/>
+      <c r="N2598" s="29"/>
+      <c r="O2598" s="29"/>
+      <c r="P2598" s="29"/>
+      <c r="Q2598" s="29"/>
+      <c r="R2598" s="29"/>
+      <c r="S2598" s="29"/>
+      <c r="T2598" s="29"/>
+      <c r="U2598" s="29"/>
+      <c r="V2598" s="29"/>
+      <c r="W2598" s="29"/>
+      <c r="X2598" s="29"/>
+      <c r="Y2598" s="29"/>
+      <c r="Z2598" s="29"/>
+      <c r="AA2598" s="29"/>
+      <c r="AB2598" s="29"/>
+      <c r="AC2598" s="29"/>
+      <c r="AD2598" s="29"/>
+      <c r="AE2598" s="29"/>
+      <c r="AF2598" s="29"/>
+      <c r="AG2598" s="29"/>
+      <c r="AH2598" s="29"/>
+    </row>
+    <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2719" s="29"/>
+      <c r="C2719" s="29"/>
+      <c r="D2719" s="29"/>
+      <c r="E2719" s="29"/>
+      <c r="F2719" s="29"/>
+      <c r="G2719" s="29"/>
+      <c r="H2719" s="29"/>
+      <c r="I2719" s="29"/>
+      <c r="J2719" s="29"/>
+      <c r="K2719" s="29"/>
+      <c r="L2719" s="29"/>
+      <c r="M2719" s="29"/>
+      <c r="N2719" s="29"/>
+      <c r="O2719" s="29"/>
+      <c r="P2719" s="29"/>
+      <c r="Q2719" s="29"/>
+      <c r="R2719" s="29"/>
+      <c r="S2719" s="29"/>
+      <c r="T2719" s="29"/>
+      <c r="U2719" s="29"/>
+      <c r="V2719" s="29"/>
+      <c r="W2719" s="29"/>
+      <c r="X2719" s="29"/>
+      <c r="Y2719" s="29"/>
+      <c r="Z2719" s="29"/>
+      <c r="AA2719" s="29"/>
+      <c r="AB2719" s="29"/>
+      <c r="AC2719" s="29"/>
+      <c r="AD2719" s="29"/>
+      <c r="AE2719" s="29"/>
+      <c r="AF2719" s="29"/>
+      <c r="AG2719" s="29"/>
+      <c r="AH2719" s="29"/>
+    </row>
+    <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2837" s="29"/>
+      <c r="C2837" s="29"/>
+      <c r="D2837" s="29"/>
+      <c r="E2837" s="29"/>
+      <c r="F2837" s="29"/>
+      <c r="G2837" s="29"/>
+      <c r="H2837" s="29"/>
+      <c r="I2837" s="29"/>
+      <c r="J2837" s="29"/>
+      <c r="K2837" s="29"/>
+      <c r="L2837" s="29"/>
+      <c r="M2837" s="29"/>
+      <c r="N2837" s="29"/>
+      <c r="O2837" s="29"/>
+      <c r="P2837" s="29"/>
+      <c r="Q2837" s="29"/>
+      <c r="R2837" s="29"/>
+      <c r="S2837" s="29"/>
+      <c r="T2837" s="29"/>
+      <c r="U2837" s="29"/>
+      <c r="V2837" s="29"/>
+      <c r="W2837" s="29"/>
+      <c r="X2837" s="29"/>
+      <c r="Y2837" s="29"/>
+      <c r="Z2837" s="29"/>
+      <c r="AA2837" s="29"/>
+      <c r="AB2837" s="29"/>
+      <c r="AC2837" s="29"/>
+      <c r="AD2837" s="29"/>
+      <c r="AE2837" s="29"/>
+      <c r="AF2837" s="29"/>
+      <c r="AG2837" s="29"/>
+      <c r="AH2837" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B87:AG87"/>
-    <mergeCell ref="B112:AH112"/>
-    <mergeCell ref="B308:AH308"/>
-    <mergeCell ref="B511:AH511"/>
-    <mergeCell ref="B712:AH712"/>
-    <mergeCell ref="B887:AH887"/>
-    <mergeCell ref="B1100:AH1100"/>
-    <mergeCell ref="B1227:AH1227"/>
-    <mergeCell ref="B1390:AH1390"/>
-    <mergeCell ref="B1502:AH1502"/>
-    <mergeCell ref="B1604:AH1604"/>
-    <mergeCell ref="B1698:AH1698"/>
-    <mergeCell ref="B1945:AH1945"/>
-    <mergeCell ref="B2031:AH2031"/>
-    <mergeCell ref="B2719:AH2719"/>
     <mergeCell ref="B2837:AH2837"/>
     <mergeCell ref="B2153:AH2153"/>
     <mergeCell ref="B2317:AH2317"/>
     <mergeCell ref="B2419:AH2419"/>
     <mergeCell ref="B2509:AH2509"/>
     <mergeCell ref="B2598:AH2598"/>
+    <mergeCell ref="B1604:AH1604"/>
+    <mergeCell ref="B1698:AH1698"/>
+    <mergeCell ref="B1945:AH1945"/>
+    <mergeCell ref="B2031:AH2031"/>
+    <mergeCell ref="B2719:AH2719"/>
+    <mergeCell ref="B887:AH887"/>
+    <mergeCell ref="B1100:AH1100"/>
+    <mergeCell ref="B1227:AH1227"/>
+    <mergeCell ref="B1390:AH1390"/>
+    <mergeCell ref="B1502:AH1502"/>
+    <mergeCell ref="B87:AG87"/>
+    <mergeCell ref="B112:AH112"/>
+    <mergeCell ref="B308:AH308"/>
+    <mergeCell ref="B511:AH511"/>
+    <mergeCell ref="B712:AH712"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -8484,16 +8471,18 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1">
         <v>2020</v>
@@ -8589,133 +8578,102 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4">
-        <f>'AEO Table 9'!C$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
-        <f>'AEO Table 9'!D$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
-        <f>'AEO Table 9'!E$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="E2" s="4">
-        <f>'AEO Table 9'!F$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
-        <f>'AEO Table 9'!G$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4">
-        <f>'AEO Table 9'!H$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4">
-        <f>'AEO Table 9'!I$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="I2" s="4">
-        <f>'AEO Table 9'!J$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="J2" s="4">
-        <f>'AEO Table 9'!K$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="K2" s="4">
-        <f>'AEO Table 9'!L$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="L2" s="4">
-        <f>'AEO Table 9'!M$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="M2" s="4">
-        <f>'AEO Table 9'!N$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="N2" s="4">
-        <f>'AEO Table 9'!O$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="O2" s="4">
-        <f>'AEO Table 9'!P$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="P2" s="4">
-        <f>'AEO Table 9'!Q$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="4">
-        <f>'AEO Table 9'!R$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="R2" s="4">
-        <f>'AEO Table 9'!S$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="S2" s="4">
-        <f>'AEO Table 9'!T$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="T2" s="4">
-        <f>'AEO Table 9'!U$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="U2" s="4">
-        <f>'AEO Table 9'!V$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="V2" s="4">
-        <f>'AEO Table 9'!W$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="W2" s="4">
-        <f>'AEO Table 9'!X$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="X2" s="4">
-        <f>'AEO Table 9'!Y$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="4">
-        <f>'AEO Table 9'!Z$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="4">
-        <f>'AEO Table 9'!AA$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="4">
-        <f>'AEO Table 9'!AB$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="4">
-        <f>'AEO Table 9'!AC$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="4">
-        <f>'AEO Table 9'!AD$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="4">
-        <f>'AEO Table 9'!AE$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="4">
-        <f>'AEO Table 9'!AF$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="4">
-        <f>'AEO Table 9'!AG$22*gigawatts_to_megawatts</f>
-        <v>22778.303</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="4"/>
     </row>

</xml_diff>